<commit_message>
Update "Fuels" sheet variables and associated structure (#232)
</commit_message>
<xml_diff>
--- a/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
+++ b/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\fuels\PEIIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\fuels\PEIIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5BDB8-164C-4260-8BDD-310BFE54C72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF141244-6611-464B-A918-1489A292BDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21225" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16110" yWindow="1005" windowWidth="31950" windowHeight="20490" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="67">
   <si>
     <t>Source:</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>jet fuel</t>
-  </si>
-  <si>
-    <t>natural gas nonpeaker</t>
   </si>
   <si>
     <t>geothermal</t>
@@ -255,6 +252,12 @@
   </si>
   <si>
     <t>Improvement Rate (dimensionless)</t>
+  </si>
+  <si>
+    <t>natural gas steam turbine</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle</t>
   </si>
 </sst>
 </file>
@@ -711,22 +714,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -734,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,92 +747,92 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +865,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
@@ -883,16 +886,16 @@
         <v>23</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1346,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
@@ -1370,13 +1373,13 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,7 +1833,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -1854,13 +1857,13 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2314,7 +2317,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -2338,13 +2341,13 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2798,7 +2801,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -2822,13 +2825,13 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3282,7 +3285,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -3306,13 +3309,13 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3766,7 +3769,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -3790,13 +3793,13 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4230,82 +4233,86 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="L1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4357,8 +4364,11 @@
       <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4410,8 +4420,11 @@
       <c r="Q3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4463,8 +4476,11 @@
       <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4516,8 +4532,11 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4569,8 +4588,11 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4622,8 +4644,11 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4675,8 +4700,11 @@
       <c r="Q8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4728,8 +4756,11 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4781,8 +4812,11 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4834,8 +4868,11 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4887,8 +4924,11 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4938,6 +4978,9 @@
         <v>0</v>
       </c>
       <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <v>0</v>
       </c>
     </row>
@@ -4971,7 +5014,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -4992,16 +5035,16 @@
         <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>